<commit_message>
adjusted stud per vak
</commit_message>
<xml_diff>
--- a/data bekijken/stud per vak.xlsx
+++ b/data bekijken/stud per vak.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tijnp\Documents\AlgHeur\crispy_waffles\data bekijken\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B13FB448-898A-4F80-833E-91F8AAE9FBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017203C5-C457-402E-89B2-9F35CFABD00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A518884E-44BB-4CFF-89E0-81CDF99B1A9C}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{A518884E-44BB-4CFF-89E0-81CDF99B1A9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Advanced Heuristics                     20.0</t>
   </si>
@@ -123,6 +123,30 @@
   </si>
   <si>
     <t>Zoeken sturen en bewegen                42.0</t>
+  </si>
+  <si>
+    <t>Students per course</t>
+  </si>
+  <si>
+    <t>Lectures</t>
+  </si>
+  <si>
+    <t>tutorial amount</t>
+  </si>
+  <si>
+    <t>tut cap</t>
+  </si>
+  <si>
+    <t>nodige tut</t>
+  </si>
+  <si>
+    <t>lab amount</t>
+  </si>
+  <si>
+    <t>lab cap</t>
+  </si>
+  <si>
+    <t>nodige labs</t>
   </si>
 </sst>
 </file>
@@ -494,160 +518,632 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC8B092E-F312-42ED-8B2D-7A43C5B21A11}">
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>25</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>20</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>40</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>20</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>40</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>40</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>15</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>10</v>
+      </c>
+      <c r="J12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>40</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>25</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>20</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>15</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>20</v>
+      </c>
+      <c r="J21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>20</v>
+      </c>
+      <c r="J22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>20</v>
+      </c>
+      <c r="J23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>15</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>15</v>
+      </c>
+      <c r="J25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>20</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>40</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>40</v>
+      </c>
+      <c r="J27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>20</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>20</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>20</v>
+      </c>
+      <c r="J29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>28</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>15</v>
+      </c>
+      <c r="J30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <f>SUM(C2:C30)</f>
+        <v>39</v>
+      </c>
+      <c r="F31">
+        <f>SUM(F2:F30)</f>
+        <v>40</v>
+      </c>
+      <c r="J31">
+        <f>SUM(J2:J30)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <f>SUM(C31,F31,J31)</f>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>